<commit_message>
feat(gen_out): add algo for generating of intertype groups weight
</commit_message>
<xml_diff>
--- a/out/log.xlsx
+++ b/out/log.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\art_home\university\mindmap\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2469256-42AF-4D0B-B526-AB25E4A4CFCC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3BB614-9E50-4418-9278-3978D8933AC8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="groups" sheetId="2" r:id="rId2"/>
-    <sheet name="Вертикальная" sheetId="3" r:id="rId3"/>
-    <sheet name="Вилы" sheetId="4" r:id="rId4"/>
-    <sheet name="Кластеринг" sheetId="5" r:id="rId5"/>
-    <sheet name="Концепт-карта" sheetId="6" r:id="rId6"/>
+    <sheet name="Вилы" sheetId="3" r:id="rId3"/>
+    <sheet name="Кластеринг" sheetId="4" r:id="rId4"/>
+    <sheet name="Концепт-карта" sheetId="5" r:id="rId5"/>
+    <sheet name="weight_by_mindmap_type" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
   <si>
     <t>чел №0</t>
   </si>
@@ -42,30 +42,30 @@
     <t>вес группы</t>
   </si>
   <si>
+    <t>Исаев</t>
+  </si>
+  <si>
+    <t>Череданов</t>
+  </si>
+  <si>
     <t>Белиовский</t>
   </si>
   <si>
-    <t>Исаев</t>
-  </si>
-  <si>
-    <t>Череданов</t>
-  </si>
-  <si>
     <t>{161, 131, 74, 15, 178, 117, 118, 247, 126}</t>
   </si>
   <si>
     <t>19.0</t>
   </si>
   <si>
+    <t>В</t>
+  </si>
+  <si>
     <t>Б</t>
   </si>
   <si>
     <t>Кателкин</t>
   </si>
   <si>
-    <t>В</t>
-  </si>
-  <si>
     <t>{74, 116, 114, 92}</t>
   </si>
   <si>
@@ -75,12 +75,12 @@
     <t>Жигалин</t>
   </si>
   <si>
+    <t>Яшков</t>
+  </si>
+  <si>
     <t>Замятин</t>
   </si>
   <si>
-    <t>Яшков</t>
-  </si>
-  <si>
     <t>{178, 42}</t>
   </si>
   <si>
@@ -90,12 +90,12 @@
     <t>З</t>
   </si>
   <si>
+    <t>Венилев</t>
+  </si>
+  <si>
     <t>Зотьева</t>
   </si>
   <si>
-    <t>Венилев</t>
-  </si>
-  <si>
     <t>{2, 103}</t>
   </si>
   <si>
@@ -105,27 +105,27 @@
     <t>Гурьянов</t>
   </si>
   <si>
+    <t>А</t>
+  </si>
+  <si>
     <t>П</t>
   </si>
   <si>
-    <t>А</t>
-  </si>
-  <si>
     <t>{51}</t>
   </si>
   <si>
     <t>1.0</t>
   </si>
   <si>
+    <t>Качалова</t>
+  </si>
+  <si>
+    <t>Д</t>
+  </si>
+  <si>
     <t>Г</t>
   </si>
   <si>
-    <t>Д</t>
-  </si>
-  <si>
-    <t>Качалова</t>
-  </si>
-  <si>
     <t>{114, 109}</t>
   </si>
   <si>
@@ -135,51 +135,51 @@
     <t>Макаренков</t>
   </si>
   <si>
+    <t>Азябин</t>
+  </si>
+  <si>
     <t>Астахенко</t>
   </si>
   <si>
-    <t>Азябин</t>
-  </si>
-  <si>
     <t>{114}</t>
   </si>
   <si>
     <t>1.3333333333333333</t>
   </si>
   <si>
+    <t>Валова</t>
+  </si>
+  <si>
+    <t>Елфимова</t>
+  </si>
+  <si>
     <t>Алиев</t>
   </si>
   <si>
-    <t>Елфимова</t>
-  </si>
-  <si>
-    <t>Валова</t>
-  </si>
-  <si>
     <t>{9}</t>
   </si>
   <si>
+    <t>Гудков</t>
+  </si>
+  <si>
     <t>Синрин</t>
   </si>
   <si>
     <t>Ермаков</t>
   </si>
   <si>
-    <t>Гудков</t>
-  </si>
-  <si>
     <t>{162, 2, 103, 156, 157}</t>
   </si>
   <si>
     <t>8.0</t>
   </si>
   <si>
+    <t>Вареница</t>
+  </si>
+  <si>
     <t>М</t>
   </si>
   <si>
-    <t>Вареница</t>
-  </si>
-  <si>
     <t>Пашинский</t>
   </si>
   <si>
@@ -204,15 +204,15 @@
     <t>2.6666666666666665</t>
   </si>
   <si>
+    <t>Чернджин</t>
+  </si>
+  <si>
     <t>Р</t>
   </si>
   <si>
     <t>Кадрилеев</t>
   </si>
   <si>
-    <t>Чернджин</t>
-  </si>
-  <si>
     <t>{103}</t>
   </si>
   <si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>{2, 155, 103}</t>
+  </si>
+  <si>
+    <t>Вертикальная</t>
+  </si>
+  <si>
+    <t>Вилы</t>
+  </si>
+  <si>
+    <t>Кластеринг</t>
+  </si>
+  <si>
+    <t>Концепт-карта</t>
   </si>
 </sst>
 </file>
@@ -585,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -597,17 +609,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -838,11 +848,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -859,6 +876,159 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -868,19 +1038,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,155 +1070,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1065,6 +1097,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1085,19 +1124,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1107,51 +1146,125 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>0.63992869875222813</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>0.45348837209302317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>0.49714285714285722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5">
+        <v>0.60984848484848486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>0.48172757475083061</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7">
+        <v>0.45153061224489788</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>0.28888888888888892</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>